<commit_message>
update seagrass protocol material
</commit_message>
<xml_diff>
--- a/assets/modules/fish-trawls/marinegeo_spreadsheet_fish_trawls.xlsx
+++ b/assets/modules/fish-trawls/marinegeo_spreadsheet_fish_trawls.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Dropbox (Smithsonian)\marinegeo_resources\protocols\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\spreadsheets_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2735C683-54FC-4031-AFFD-94509556F5DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F03B19-E526-4390-8912-1FF31BC28557}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>data_entry_year</t>
   </si>
   <si>
-    <t>v0.4.0</t>
-  </si>
-  <si>
     <t>sample_metadata_notes</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total abundance of each fish taxon. </t>
+  </si>
+  <si>
+    <t>v0.5.0</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1195,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="161.1" customHeight="1">
       <c r="B1" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1253,7 +1253,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1397,13 +1397,13 @@
         <v>49</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N1" s="29" t="s">
         <v>55</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1708,16 +1708,16 @@
         <v>64</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>83</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2007,16 +2007,16 @@
         <v>64</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>83</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2472,10 +2472,10 @@
         <v>63</v>
       </c>
       <c r="B25" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>0</v>
@@ -2491,7 +2491,7 @@
         <v>55</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>0</v>
@@ -2504,10 +2504,10 @@
         <v>63</v>
       </c>
       <c r="B27" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>0</v>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="28" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
       <c r="A28" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="14" t="s">
@@ -2529,7 +2529,7 @@
     </row>
     <row r="29" spans="1:6" s="16" customFormat="1" ht="63">
       <c r="A29" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>75</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="30" spans="1:6" s="16" customFormat="1" ht="47.25">
       <c r="A30" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>44</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="31" spans="1:6" s="16" customFormat="1" ht="31.5">
       <c r="A31" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>43</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="32" spans="1:6" s="16" customFormat="1" ht="31.5">
       <c r="A32" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>64</v>
@@ -2597,13 +2597,13 @@
     </row>
     <row r="33" spans="1:6" s="34" customFormat="1" ht="66" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>0</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="34" spans="1:6" s="34" customFormat="1" ht="66" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>0</v>
@@ -2629,13 +2629,13 @@
     </row>
     <row r="35" spans="1:6" s="16" customFormat="1" ht="96" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -2643,13 +2643,13 @@
     </row>
     <row r="36" spans="1:6" s="16" customFormat="1" ht="96" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>0</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="37" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
       <c r="A37" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="14" t="s">
@@ -2671,7 +2671,7 @@
     </row>
     <row r="38" spans="1:6" s="16" customFormat="1" ht="63">
       <c r="A38" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>75</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="39" spans="1:6" s="16" customFormat="1" ht="47.25">
       <c r="A39" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>44</v>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="40" spans="1:6" s="16" customFormat="1" ht="31.5">
       <c r="A40" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="38" t="s">
         <v>43</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="41" spans="1:6" s="16" customFormat="1" ht="31.5">
       <c r="A41" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>64</v>
@@ -2739,13 +2739,13 @@
     </row>
     <row r="42" spans="1:6" s="34" customFormat="1" ht="66" customHeight="1">
       <c r="A42" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>0</v>
@@ -2755,13 +2755,13 @@
     </row>
     <row r="43" spans="1:6" s="34" customFormat="1" ht="66" customHeight="1">
       <c r="A43" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>0</v>
@@ -2771,13 +2771,13 @@
     </row>
     <row r="44" spans="1:6" s="16" customFormat="1" ht="96" customHeight="1">
       <c r="A44" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="39" t="s">
         <v>51</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
@@ -2787,13 +2787,13 @@
     </row>
     <row r="45" spans="1:6" s="16" customFormat="1" ht="96" customHeight="1">
       <c r="A45" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>0</v>

</xml_diff>